<commit_message>
changes supporting specification of integration of PCAP feeds
</commit_message>
<xml_diff>
--- a/xlsxPCES/examples/flows.xlsx
+++ b/xlsxPCES/examples/flows.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicol/Dropbox/github-repos/pcesbld/xlsxPCES/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437B2323-7501-784B-B7D7-B4D12A789E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A21854-1854-DB40-928F-A8FEEE03AB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2820" windowWidth="34200" windowHeight="16920" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
+    <workbookView xWindow="6520" yWindow="11940" windowWidth="34200" windowHeight="20240" xr2:uid="{7E753834-245C-A346-8630-DEF93455D7FF}"/>
   </bookViews>
   <sheets>
     <sheet name="topo" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="netParams" sheetId="5" r:id="rId5"/>
     <sheet name="experiments" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -1571,17 +1572,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95325CDA-052A-9A47-A8FD-348C19C2091E}">
   <dimension ref="A2:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
     <col min="8" max="8" width="8.83203125" customWidth="1"/>

</xml_diff>